<commit_message>
real final commit, url 통합
</commit_message>
<xml_diff>
--- a/w_file/물 비율.xlsx
+++ b/w_file/물 비율.xlsx
@@ -4868,11 +4868,11 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>600t</t>
+          <t>995t</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="223">

</xml_diff>